<commit_message>
📊 Dados MIBGAS atualizados automaticamente
</commit_message>
<xml_diff>
--- a/Tarifarios_🔥_Gas_Natural_Tiago_Felicia.xlsx
+++ b/Tarifarios_🔥_Gas_Natural_Tiago_Felicia.xlsx
@@ -14946,7 +14946,7 @@
         <v>45931</v>
       </c>
       <c r="B641" t="n">
-        <v>31.4</v>
+        <v>30.83</v>
       </c>
     </row>
     <row r="642">
@@ -21555,7 +21555,7 @@
         </is>
       </c>
       <c r="B2" s="8" t="n">
-        <v>45930</v>
+        <v>45931</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
🔥 Dados MIBGAS atualizados automaticamente
</commit_message>
<xml_diff>
--- a/Tarifarios_🔥_Gas_Natural_Tiago_Felicia.xlsx
+++ b/Tarifarios_🔥_Gas_Natural_Tiago_Felicia.xlsx
@@ -15389,7 +15389,7 @@
         <v>45985</v>
       </c>
       <c r="B695" t="n">
-        <v>30.28</v>
+        <v>30.35</v>
       </c>
     </row>
     <row r="696">
@@ -15397,7 +15397,7 @@
         <v>45986</v>
       </c>
       <c r="B696" t="n">
-        <v>30.28</v>
+        <v>30.35</v>
       </c>
     </row>
     <row r="697">
@@ -15405,7 +15405,7 @@
         <v>45987</v>
       </c>
       <c r="B697" t="n">
-        <v>30.28</v>
+        <v>30.35</v>
       </c>
     </row>
     <row r="698">
@@ -15413,7 +15413,7 @@
         <v>45988</v>
       </c>
       <c r="B698" t="n">
-        <v>30.28</v>
+        <v>30.35</v>
       </c>
     </row>
     <row r="699">
@@ -15421,7 +15421,7 @@
         <v>45989</v>
       </c>
       <c r="B699" t="n">
-        <v>30.28</v>
+        <v>30.35</v>
       </c>
     </row>
     <row r="700">
@@ -15429,7 +15429,7 @@
         <v>45990</v>
       </c>
       <c r="B700" t="n">
-        <v>30.28</v>
+        <v>30.35</v>
       </c>
     </row>
     <row r="701">
@@ -15437,7 +15437,7 @@
         <v>45991</v>
       </c>
       <c r="B701" t="n">
-        <v>30.28</v>
+        <v>30.35</v>
       </c>
     </row>
     <row r="702">

</xml_diff>